<commit_message>
further updates to naming, diagram parity, and signals spreadsheet update
</commit_message>
<xml_diff>
--- a/SAT_Solver_Signals.xlsx
+++ b/SAT_Solver_Signals.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="182">
   <si>
     <t>Device</t>
   </si>
@@ -43,297 +43,309 @@
     <t>input</t>
   </si>
   <si>
+    <t>clk_i</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>rst_i</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>[CLAUSE_WIDTH * CLAUSE_COUNT - 1 : 0]</t>
+  </si>
+  <si>
+    <t>clauses_i</t>
+  </si>
+  <si>
+    <t>clause input</t>
+  </si>
+  <si>
+    <t>control/data</t>
+  </si>
+  <si>
+    <t>[CLAUSE_COUNT - 1 : 0]</t>
+  </si>
+  <si>
+    <t>clause_valid_i</t>
+  </si>
+  <si>
+    <t>valid clause indication</t>
+  </si>
+  <si>
+    <t>wr_en_i</t>
+  </si>
+  <si>
+    <t>write enable</t>
+  </si>
+  <si>
+    <t>rd_en_i</t>
+  </si>
+  <si>
+    <t>read enable</t>
+  </si>
+  <si>
+    <t>cOF_i</t>
+  </si>
+  <si>
+    <t>clear overflow flag</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>empty_o</t>
+  </si>
+  <si>
+    <t>fifo_last empty flag</t>
+  </si>
+  <si>
+    <t>OF_o</t>
+  </si>
+  <si>
+    <t>overflow flag</t>
+  </si>
+  <si>
+    <t>[CLAUSE_WIDTH - 1 : 0]</t>
+  </si>
+  <si>
+    <t>clause_o</t>
+  </si>
+  <si>
+    <t>clause output</t>
+  </si>
+  <si>
+    <t>Variable_Table_Cluster</t>
+  </si>
+  <si>
+    <t>axi_control</t>
+  </si>
+  <si>
+    <t>axi_en_i</t>
+  </si>
+  <si>
+    <t>axi enable</t>
+  </si>
+  <si>
+    <t>axi_wr_en_i</t>
+  </si>
+  <si>
+    <t>axi write enable</t>
+  </si>
+  <si>
+    <t>axi_data</t>
+  </si>
+  <si>
+    <t>[VARIABLE_ADDRESS_WIDTH - 1 : 0]</t>
+  </si>
+  <si>
+    <t>axi_addr_i</t>
+  </si>
+  <si>
+    <t>axi address input</t>
+  </si>
+  <si>
+    <t>axi_data_i</t>
+  </si>
+  <si>
+    <t>axi data input</t>
+  </si>
+  <si>
+    <t>en_i</t>
+  </si>
+  <si>
+    <t>runtime enable</t>
+  </si>
+  <si>
+    <t>runtime write enable</t>
+  </si>
+  <si>
+    <t>[CLUSTER_SIZE * VARIABLE_ADDRESS_WIDTH - 1 : 0]</t>
+  </si>
+  <si>
+    <t>addr_mi</t>
+  </si>
+  <si>
+    <t>runtime multi address port</t>
+  </si>
+  <si>
+    <t>data_i</t>
+  </si>
+  <si>
+    <t>runtime data input</t>
+  </si>
+  <si>
+    <t>[CLUSTER_SIZE - 1 : 0]</t>
+  </si>
+  <si>
+    <t>data_mo</t>
+  </si>
+  <si>
+    <t>runtime multi data output</t>
+  </si>
+  <si>
+    <t>Clause_Evaluator_Cluster</t>
+  </si>
+  <si>
+    <t>[((NSAT - REDUCE) * CLUSTER_SIZE - 1) : 0]</t>
+  </si>
+  <si>
+    <t>var_val_mi</t>
+  </si>
+  <si>
+    <t>variable value multiple input</t>
+  </si>
+  <si>
+    <t>var_neg_mi</t>
+  </si>
+  <si>
+    <t>variable negation multiple input</t>
+  </si>
+  <si>
+    <t>break_mo</t>
+  </si>
+  <si>
+    <t>break value multiple output</t>
+  </si>
+  <si>
+    <t>Clause_Evaluator_2</t>
+  </si>
+  <si>
+    <t>[(NSAT - REDUCE) - 1 : 0]</t>
+  </si>
+  <si>
+    <t>var_val_i</t>
+  </si>
+  <si>
+    <t>variable value input</t>
+  </si>
+  <si>
+    <t>var_neg_i</t>
+  </si>
+  <si>
+    <t>variable negation input</t>
+  </si>
+  <si>
+    <t>break_o</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Temporal_Buffer_Wrapper</t>
+  </si>
+  <si>
+    <t>[NSAT_BITS-1:0]</t>
+  </si>
+  <si>
+    <t>wr_index_i</t>
+  </si>
+  <si>
+    <t>which flip is currently being evaluated</t>
+  </si>
+  <si>
+    <t>[(NSAT - 1) * MC * LAW - 1 : 0]</t>
+  </si>
+  <si>
+    <t>wr_literals_mi</t>
+  </si>
+  <si>
+    <t>literals from clause table for each flip</t>
+  </si>
+  <si>
+    <t>rd_index_i</t>
+  </si>
+  <si>
+    <t>which flip was selected by the heuristic selector</t>
+  </si>
+  <si>
+    <t>literals_mo</t>
+  </si>
+  <si>
+    <t>literals from clause table for selected flip</t>
+  </si>
+  <si>
+    <t>Address_Translation_Table</t>
+  </si>
+  <si>
+    <t>[LITERAL_ADDRESS_WIDTH:0]</t>
+  </si>
+  <si>
+    <t>axi_wr_addr_i</t>
+  </si>
+  <si>
+    <t>axi write address</t>
+  </si>
+  <si>
+    <t>[CLAUSE_TABLE_ADDRESS_WIDTH + CLAUSE_COUNT - 1 : 0]</t>
+  </si>
+  <si>
+    <t>axi_wr_data_i</t>
+  </si>
+  <si>
+    <t>rd_addr_i</t>
+  </si>
+  <si>
+    <t>read address</t>
+  </si>
+  <si>
+    <t>[CLAUSE_TABLE_ADDRESS_WIDTH - 1:0]</t>
+  </si>
+  <si>
+    <t>addr_o</t>
+  </si>
+  <si>
+    <t>address output for clause table</t>
+  </si>
+  <si>
+    <t>[CLAUSE_COUNT-1:0]</t>
+  </si>
+  <si>
+    <t>mask_o</t>
+  </si>
+  <si>
+    <t>mask valid bits</t>
+  </si>
+  <si>
+    <t>Clause_Register</t>
+  </si>
+  <si>
+    <t>[LITERAL_ADDRESS_WIDTH * NSAT - 1 : 0]</t>
+  </si>
+  <si>
+    <t>data input</t>
+  </si>
+  <si>
+    <t>data_o</t>
+  </si>
+  <si>
+    <t>data output</t>
+  </si>
+  <si>
+    <t>Clause_Table</t>
+  </si>
+  <si>
     <t>clk</t>
   </si>
   <si>
-    <t>control</t>
-  </si>
-  <si>
-    <t>reset</t>
-  </si>
-  <si>
-    <t>[CLAUSE_COUNT - 1 : 0]</t>
-  </si>
-  <si>
-    <t>clause_valid_i</t>
-  </si>
-  <si>
-    <t>valid clause indication</t>
-  </si>
-  <si>
-    <t>wren</t>
-  </si>
-  <si>
-    <t>write enable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rden </t>
-  </si>
-  <si>
-    <t>read enable</t>
-  </si>
-  <si>
-    <t>cOF</t>
-  </si>
-  <si>
-    <t>clear overflow flag</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>empty</t>
-  </si>
-  <si>
-    <t>fifo_last empty flag</t>
-  </si>
-  <si>
-    <t>OF</t>
-  </si>
-  <si>
-    <t>overflow flag</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>[CLAUSE_WIDTH * CLAUSE_COUNT - 1 : 0]</t>
-  </si>
-  <si>
-    <t>clauses_i</t>
-  </si>
-  <si>
-    <t>clause input</t>
-  </si>
-  <si>
-    <t>[CLAUSE_WIDTH - 1 : 0]</t>
-  </si>
-  <si>
-    <t>clause_o</t>
-  </si>
-  <si>
-    <t>clause output</t>
-  </si>
-  <si>
-    <t>Variable_Table_Cluster</t>
-  </si>
-  <si>
-    <t>clk_i</t>
-  </si>
-  <si>
-    <t>en_i</t>
-  </si>
-  <si>
-    <t>runtime enable</t>
-  </si>
-  <si>
-    <t>wr_en_i</t>
-  </si>
-  <si>
-    <t>runtime write enable</t>
-  </si>
-  <si>
-    <t>[CLUSTER_SIZE * VARIABLE_ADDRESS_WIDTH - 1 : 0]</t>
-  </si>
-  <si>
-    <t>addr_mi</t>
-  </si>
-  <si>
-    <t>runtime multi address port</t>
-  </si>
-  <si>
-    <t>data_i</t>
-  </si>
-  <si>
-    <t>runtime data input</t>
-  </si>
-  <si>
-    <t>[CLUSTER_SIZE - 1 : 0]</t>
-  </si>
-  <si>
-    <t>data_mo</t>
-  </si>
-  <si>
-    <t>runtime multi data output</t>
-  </si>
-  <si>
-    <t>axi_control</t>
-  </si>
-  <si>
-    <t>axi_en_i</t>
-  </si>
-  <si>
-    <t>axi enable</t>
-  </si>
-  <si>
-    <t>axi_wr_en_i</t>
-  </si>
-  <si>
-    <t>axi write enable</t>
-  </si>
-  <si>
-    <t>axi_data</t>
-  </si>
-  <si>
-    <t>[VARIABLE_ADDRESS_WIDTH - 1 : 0]</t>
-  </si>
-  <si>
-    <t>axi_addr_i</t>
-  </si>
-  <si>
-    <t>axi address input</t>
-  </si>
-  <si>
-    <t>axi_data_i</t>
-  </si>
-  <si>
-    <t>axi data input</t>
-  </si>
-  <si>
-    <t>Clause_Evaluator_Cluster</t>
-  </si>
-  <si>
-    <t>reset_i</t>
-  </si>
-  <si>
-    <t>[((NSAT - REDUCE) * CLUSTER_SIZE - 1) : 0]</t>
-  </si>
-  <si>
-    <t>var_val_i</t>
-  </si>
-  <si>
-    <t>variable value input</t>
-  </si>
-  <si>
-    <t>var_neg_i</t>
-  </si>
-  <si>
-    <t>variable negation input</t>
-  </si>
-  <si>
-    <t>break_o</t>
-  </si>
-  <si>
-    <t>break truth value</t>
-  </si>
-  <si>
-    <t>Temporal_Buffer_Wrapper</t>
-  </si>
-  <si>
-    <t>[NSAT_BITS-1:0]</t>
-  </si>
-  <si>
-    <t>write_index_i</t>
-  </si>
-  <si>
-    <t>which flip is currently being evaluated</t>
-  </si>
-  <si>
-    <t>write_en_i</t>
-  </si>
-  <si>
-    <t>[(NSAT-1)*MCPV*(LAW+1)-1:0]</t>
-  </si>
-  <si>
-    <t>literals_multi_i</t>
-  </si>
-  <si>
-    <t>literals from clause table for each flip</t>
-  </si>
-  <si>
-    <t>read_index_i</t>
-  </si>
-  <si>
-    <t>which flip was selected by the heuristic selector</t>
-  </si>
-  <si>
-    <t>literals_multi_o</t>
-  </si>
-  <si>
-    <t>literals from clause table for selected flip</t>
-  </si>
-  <si>
-    <t>Address_Translation_Table</t>
-  </si>
-  <si>
-    <t>[LITERAL_ADDRESS_WIDTH:0]</t>
-  </si>
-  <si>
-    <t>wr_addr_i</t>
-  </si>
-  <si>
-    <t>write address</t>
-  </si>
-  <si>
-    <t>rd_addr_i</t>
-  </si>
-  <si>
-    <t>read address</t>
-  </si>
-  <si>
-    <t>[CLAUSE_TABLE_ADDRESS_WIDTH + CLAUSE_COUNT - 1 : 0]</t>
-  </si>
-  <si>
-    <t>wr_data_i</t>
-  </si>
-  <si>
-    <t>data input</t>
-  </si>
-  <si>
-    <t>[CLAUSE_TABLE_ADDRESS_WIDTH - 1:0]</t>
-  </si>
-  <si>
-    <t>addr_o</t>
-  </si>
-  <si>
-    <t>address output for clause table</t>
-  </si>
-  <si>
-    <t>[CLAUSE_COUNT-1:0]</t>
-  </si>
-  <si>
-    <t>mask_o</t>
-  </si>
-  <si>
-    <t>mask valid bits</t>
-  </si>
-  <si>
-    <t>Clause_Register</t>
-  </si>
-  <si>
-    <t>rst_i</t>
-  </si>
-  <si>
-    <t>[LITERAL_ADDRESS_WIDTH * NSAT - 1 : 0]</t>
-  </si>
-  <si>
-    <t>data_o</t>
-  </si>
-  <si>
-    <t>data output</t>
-  </si>
-  <si>
-    <t>Clause_Table</t>
-  </si>
-  <si>
-    <t>we</t>
-  </si>
-  <si>
     <t>[LITERAL_ADDRESS_WIDTH-1:0]</t>
   </si>
   <si>
-    <t>waddr</t>
+    <t>[(LITERAL_ADDRESS_WIDTH + 1) * (NSAT - 1) * CLAUSE_COUNT - 1 : 0]</t>
+  </si>
+  <si>
+    <t>axi_wr_clauses_i</t>
   </si>
   <si>
     <t>[LITERAL_ADDRESS_WIDTH-1:1]</t>
   </si>
   <si>
-    <t>raddr</t>
-  </si>
-  <si>
-    <t>[(LITERAL_ADDRESS_WIDTH + 1) * (NSAT - 1) * CLAUSE_COUNT - 1 : 0]</t>
-  </si>
-  <si>
     <t>clauses_o</t>
   </si>
   <si>
@@ -424,9 +436,6 @@
     <t>lfsr_prng</t>
   </si>
   <si>
-    <t>out</t>
-  </si>
-  <si>
     <t>prng output</t>
   </si>
   <si>
@@ -466,13 +475,10 @@
     <t>rng input</t>
   </si>
   <si>
-    <t>[$clog2(NSAT) - 1 : 0]</t>
-  </si>
-  <si>
-    <t>wren_i</t>
-  </si>
-  <si>
-    <t>wren index</t>
+    <t>[NSAT_BITS - 1 : 0]</t>
+  </si>
+  <si>
+    <t>write enable index</t>
   </si>
   <si>
     <t>selected_o</t>
@@ -481,10 +487,79 @@
     <t>selected variable numeral output</t>
   </si>
   <si>
-    <t>clause_broken_bits_o</t>
-  </si>
-  <si>
-    <t>clause broken bits output</t>
+    <t>clause_valid_bits_o</t>
+  </si>
+  <si>
+    <t>clause valid bits output</t>
+  </si>
+  <si>
+    <t>Unsat_Clause_Selector</t>
+  </si>
+  <si>
+    <t>setup_i</t>
+  </si>
+  <si>
+    <t>axi setup signal</t>
+  </si>
+  <si>
+    <t>ready_o</t>
+  </si>
+  <si>
+    <t>axi ready signal (unused)</t>
+  </si>
+  <si>
+    <t>ucb_setup_wr_en_i</t>
+  </si>
+  <si>
+    <t>axi ucb write enable access</t>
+  </si>
+  <si>
+    <t>[BUF_ADDR_WIDTH - 1 : 0]</t>
+  </si>
+  <si>
+    <t>ucb_setup_addr_i</t>
+  </si>
+  <si>
+    <t>axi ucb address access</t>
+  </si>
+  <si>
+    <t>[NSAT * LITERAL_ADDRESS_WIDTH - 1 : 0]</t>
+  </si>
+  <si>
+    <t>ucb_setup_data_i</t>
+  </si>
+  <si>
+    <t>axi ucb data access</t>
+  </si>
+  <si>
+    <t>request_i</t>
+  </si>
+  <si>
+    <t>control signal to request unsatisfied clause</t>
+  </si>
+  <si>
+    <t>write_disable_i</t>
+  </si>
+  <si>
+    <t>clear_debug_DIV_BY_ZERO_i</t>
+  </si>
+  <si>
+    <t>debug_DIV_BY_ZERO_o</t>
+  </si>
+  <si>
+    <t>fifo_empty_i</t>
+  </si>
+  <si>
+    <t>fifo_clause_i</t>
+  </si>
+  <si>
+    <t>[31 : 0]</t>
+  </si>
+  <si>
+    <t>buffer_count_o</t>
+  </si>
+  <si>
+    <t>ucb_overflow_o</t>
   </si>
 </sst>
 </file>
@@ -492,13 +567,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -549,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -563,10 +644,19 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -877,18 +967,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="59.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="48.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="22.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="59.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="48.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -948,7 +1038,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -956,19 +1046,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -976,22 +1066,22 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4">
-        <v>1</v>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1005,13 +1095,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1025,13 +1115,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1039,19 +1129,19 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1059,61 +1149,61 @@
         <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>34</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -1125,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>7</v>
@@ -1133,10 +1223,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>8</v>
@@ -1144,19 +1234,19 @@
       <c r="D13" s="4">
         <v>1</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>36</v>
+      <c r="E13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>8</v>
@@ -1164,39 +1254,39 @@
       <c r="D14" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>37</v>
+      <c r="E14" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>41</v>
+      <c r="D15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
@@ -1205,104 +1295,104 @@
         <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+        <v>46</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="E19" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F19" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="5" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>56</v>
@@ -1311,7 +1401,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
@@ -1325,13 +1415,13 @@
         <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
         <v>58</v>
       </c>
@@ -1345,75 +1435,75 @@
         <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>7</v>
@@ -1433,7 +1523,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>10</v>
@@ -1448,132 +1538,132 @@
         <v>11</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="4">
-        <v>1</v>
-      </c>
       <c r="E30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="3" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="A32" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="B32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="C33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>10</v>
@@ -1585,201 +1675,201 @@
         <v>1</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="F36" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>88</v>
+        <v>8</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>91</v>
+        <v>8</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="4">
-        <v>1</v>
+      <c r="D41" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="4">
-        <v>1</v>
+      <c r="D42" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="4">
-        <v>1</v>
+      <c r="D43" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F44" s="3" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>96</v>
@@ -1825,10 +1915,10 @@
         <v>1</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -1836,19 +1926,19 @@
         <v>99</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>101</v>
+      <c r="D48" s="4">
+        <v>1</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
@@ -1856,19 +1946,19 @@
         <v>99</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
@@ -1876,47 +1966,47 @@
         <v>99</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="F51" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>8</v>
@@ -1925,98 +2015,98 @@
         <v>1</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>110</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="4">
-        <v>1</v>
+      <c r="D53" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="4">
-        <v>1</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="F54" s="3" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="4">
-        <v>1</v>
+      <c r="D55" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="4">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>8</v>
@@ -2025,315 +2115,315 @@
         <v>1</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>121</v>
+      <c r="D58" s="4">
+        <v>1</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="4" t="s">
-        <v>121</v>
+      <c r="D59" s="4">
+        <v>1</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>126</v>
+      <c r="D60" s="4">
+        <v>1</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>126</v>
+      <c r="D61" s="4">
+        <v>1</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>126</v>
+        <v>8</v>
+      </c>
+      <c r="D62" s="4">
+        <v>1</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D63" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="F63" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="3" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="4">
-        <v>1</v>
+      <c r="D64" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="4">
-        <v>1</v>
+      <c r="D65" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="3" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D66" s="4">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="3" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="4">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="4">
-        <v>1</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="4" t="s">
-        <v>139</v>
+      <c r="D69" s="4">
+        <v>1</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>141</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>139</v>
+      <c r="D70" s="4">
+        <v>1</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>144</v>
+        <v>27</v>
+      </c>
+      <c r="D71" s="4">
+        <v>32</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D72" s="4" t="s">
-        <v>147</v>
+      <c r="D72" s="4">
+        <v>1</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>148</v>
+        <v>9</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>10</v>
@@ -2341,55 +2431,477 @@
       <c r="C73" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>150</v>
+      <c r="D73" s="4">
+        <v>1</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>151</v>
+        <v>11</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>152</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+      <c r="A76" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+      <c r="A77" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+      <c r="A78" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D75" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E75" s="3" t="s">
+      <c r="F78" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+      <c r="A79" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F79" s="3" t="s">
         <v>156</v>
       </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+      <c r="A80" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+      <c r="A81" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="7">
+        <v>1</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+      <c r="A82" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="7">
+        <v>1</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+      <c r="A83" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="7">
+        <v>1</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+      <c r="A84" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="7">
+        <v>1</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+      <c r="A85" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="7">
+        <v>1</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+      <c r="A86" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+      <c r="A87" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+      <c r="A88" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="7">
+        <v>1</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+      <c r="A89" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="7">
+        <v>1</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F89" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+      <c r="A90" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" s="7">
+        <v>1</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F90" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+      <c r="A91" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91" s="7">
+        <v>1</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F91" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+      <c r="A92" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="7">
+        <v>1</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F92" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+      <c r="A93" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F93" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+      <c r="A94" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F94" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+      <c r="A95" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F95" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+      <c r="A96" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F96" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+      <c r="A97" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D97" s="7">
+        <v>1</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F97" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added function description to signal spreadsheet
</commit_message>
<xml_diff>
--- a/SAT_Solver_Signals.xlsx
+++ b/SAT_Solver_Signals.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="191">
   <si>
     <t>Device</t>
   </si>
@@ -541,25 +541,52 @@
     <t>write_disable_i</t>
   </si>
   <si>
+    <t>control signal handled within the circuit (not controller)</t>
+  </si>
+  <si>
     <t>clear_debug_DIV_BY_ZERO_i</t>
   </si>
   <si>
+    <t>debug clear control signal</t>
+  </si>
+  <si>
     <t>debug_DIV_BY_ZERO_o</t>
   </si>
   <si>
+    <t>debug flag signal</t>
+  </si>
+  <si>
     <t>fifo_empty_i</t>
   </si>
   <si>
+    <t>fifo information relayed to determine module function</t>
+  </si>
+  <si>
     <t>fifo_clause_i</t>
   </si>
   <si>
+    <t>fifo data input to the unsat clause buffer</t>
+  </si>
+  <si>
     <t>[31 : 0]</t>
   </si>
   <si>
+    <t>random input for clause selection</t>
+  </si>
+  <si>
     <t>buffer_count_o</t>
   </si>
   <si>
+    <t>how many unsat clauses are currently in the buffer</t>
+  </si>
+  <si>
+    <t>selected clause output</t>
+  </si>
+  <si>
     <t>ucb_overflow_o</t>
+  </si>
+  <si>
+    <t>ucb overflow flag</t>
   </si>
 </sst>
 </file>
@@ -2757,7 +2784,9 @@
       <c r="E89" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="F89" s="8"/>
+      <c r="F89" s="8" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="8" t="s">
@@ -2773,9 +2802,11 @@
         <v>1</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="F90" s="8"/>
+        <v>176</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="8" t="s">
@@ -2791,9 +2822,11 @@
         <v>1</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F91" s="8"/>
+        <v>178</v>
+      </c>
+      <c r="F91" s="8" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="8" t="s">
@@ -2809,9 +2842,11 @@
         <v>1</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F92" s="8"/>
+        <v>180</v>
+      </c>
+      <c r="F92" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="8" t="s">
@@ -2827,9 +2862,11 @@
         <v>169</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="F93" s="8"/>
+        <v>182</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="8" t="s">
@@ -2842,12 +2879,14 @@
         <v>8</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="F94" s="8"/>
+      <c r="F94" s="8" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="8" t="s">
@@ -2863,9 +2902,11 @@
         <v>166</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F95" s="8"/>
+        <v>186</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="8" t="s">
@@ -2883,7 +2924,9 @@
       <c r="E96" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="F96" s="8"/>
+      <c r="F96" s="8" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="8" t="s">
@@ -2899,9 +2942,11 @@
         <v>1</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F97" s="8"/>
+        <v>189</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>190</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>